<commit_message>
[doc] add 03_week_plan_kdh.xlsx update 03_week_plan_ljj.xlsx
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/03_week_plan_ljj.xlsx
+++ b/doc/_meeting_weekly_doc/03_week_plan_ljj.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,6 +34,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>세부목표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>월</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -66,16 +70,107 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>11.7 ~ 11.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 충돌 처리 구현(캐릭터 vs 캐릭터, 캐릭터 vs 오브젝트)
+* 1인칭 총 발사 모델 익스포트, 렌더링 구현
+* 건물 익스포트, 렌더링 구현
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>이재준</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11.7 ~ 11.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 충돌처리(오브젝트 vs 오브젝트, 오브젝트 vs 캐릭터)
-* 1인칭 발사(샷건) 동작 구현. 스코어 시스템 구현</t>
+    <t xml:space="preserve">* 게임순서도 작성함.
+* 메인게임 구조 변경함(인트로, 싱글게임등 클래스 추가에 스테이트 패턴 적용). 
+* 바운딩 박스 클래스 추가함
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 바운딩박스 렌더링. 충돌 처리 테스트. 주인공등 3인칭 모델 추출.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 2차 발표에 툴도 시연하니까 툴도 작업이 필요하다. 할것이 많고 사용할 수 있는 시간이 한정되어서.. 효율적으로 시간 사용 필요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 등원못함(집안일)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 바운딩박스 렌더링. 충돌 처리 테스트.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 없음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 바운딩박스 렌더링. 충돌 처리 테스트(obb vs obb)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 박스끼리 충돌시 미끌리게 처리(Sliding vector 처리).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 연구소 건물 export를 고민하고 있는데. 쓰려고 했던 모델이 정점이 많아 프레임수가 많이 떨어진다. 정점이 적은 모델로 찾아보고 있다.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 박스끼리 충돌시 미끌리게 처리. 구현 완료 하지 못함. 디버깅 필요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 모델 익스포트(1인칭,3인칭), 오브젝트 익스포트(건물)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 충돌처리 완료하지 못해서 캐릭터 파트 일을 못하고 있는데. 내일은 캐릭터 작업을 중점적으로 해야겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* (재택) 연구소, 드랍십, 우주선, 차량 등 오브젝트 export 함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 금주에 작업을 많이 못하였는데. 차주에는 작업시간을 늘려야 겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 좀비 모델 export (Idle, attack등)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1인칭 총알 발사 충돌 구현(Ray Vs OBB). 1인칭 총 발사모델 export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좀비모델 + AI연동, 남,여 카메라 전환 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sound 리소스 추가(배경음, 총소리), Tool 기능 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차 데모 준비(문서, 실행 버전등.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차 데모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 1인칭 총알 발사 충돌 구현, 데모 버전 준비</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,15 +524,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -512,17 +598,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -707,6 +782,32 @@
       </left>
       <right/>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -720,43 +821,43 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -778,10 +879,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -799,13 +900,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -826,50 +927,77 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -879,15 +1007,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1188,8 +1307,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1202,7 +1321,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
       <c r="A1" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1218,7 +1337,7 @@
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="32"/>
@@ -1249,223 +1368,259 @@
         <v>3</v>
       </c>
       <c r="B4" s="20"/>
-      <c r="C4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>4</v>
+      </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="28"/>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A5" s="38">
-        <v>42681</v>
+    <row r="5" spans="1:8" ht="52.5" customHeight="1" thickTop="1">
+      <c r="A5" s="39">
+        <v>42674</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A7" s="41"/>
+      <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="48"/>
+    </row>
+    <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A8" s="42">
+        <v>42675</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+    </row>
+    <row r="9" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A9" s="43"/>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A10" s="44"/>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="48"/>
+    </row>
+    <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A11" s="42">
+        <v>42676</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
+    </row>
+    <row r="12" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A12" s="43"/>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A13" s="44"/>
+      <c r="B13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
+    </row>
+    <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A14" s="42">
+        <v>42677</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+    </row>
+    <row r="15" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A15" s="43"/>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="54"/>
+    </row>
+    <row r="16" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A16" s="44"/>
+      <c r="B16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="48"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" thickTop="1">
+      <c r="A17" s="40">
+        <v>42678</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
+    </row>
+    <row r="18" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A18" s="40"/>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="54"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A19" s="45"/>
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61"/>
+    </row>
+    <row r="20" spans="1:8" ht="32.25" customHeight="1">
+      <c r="A20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="40"/>
-      <c r="B7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
-    </row>
-    <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="41">
-        <v>42682</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-    </row>
-    <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="42"/>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
-    </row>
-    <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="41">
-        <v>42683</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
-    </row>
-    <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="42"/>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-    </row>
-    <row r="13" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="41">
-        <v>42684</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="42"/>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
-    </row>
-    <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
-    </row>
-    <row r="17" spans="1:8" ht="18" thickTop="1">
-      <c r="A17" s="39">
-        <v>42685</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="39"/>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
-    </row>
-    <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="44"/>
-      <c r="B19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
-    </row>
-    <row r="20" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A20" s="34" t="s">
-        <v>9</v>
-      </c>
       <c r="B20" s="35"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="55"/>
+      <c r="C20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
-        <v>42688</v>
+        <v>42681</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="12"/>
+        <v>5</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1474,12 +1629,14 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
-        <v>42689</v>
+        <v>42682</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1488,12 +1645,14 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
-        <v>42690</v>
+        <v>42683</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1502,12 +1661,14 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
-        <v>42691</v>
+        <v>42684</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1516,12 +1677,14 @@
     </row>
     <row r="25" spans="1:8" ht="17.25" thickBot="1">
       <c r="A25" s="8">
-        <v>42692</v>
+        <v>42685</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
@@ -1533,12 +1696,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C6:H6"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C18:H18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:A7"/>
@@ -1554,7 +1717,7 @@
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C18:H18"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C3:H3"/>

</xml_diff>